<commit_message>
update to using zol v1.4.1
</commit_message>
<xml_diff>
--- a/Code_For_Figures_and_Analysis/Aflavus_BGCs_Analysis_Data/aflatoxin/zol/Final_Results/Consolidated_Report.xlsx
+++ b/Code_For_Figures_and_Analysis/Aflavus_BGCs_Analysis_Data/aflatoxin/zol/Final_Results/Consolidated_Report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="280">
   <si>
     <t>Data Dictionary describing columns of "Overview" spreadsheets can be found on zol's Wiki page at:</t>
   </si>
@@ -278,16 +278,16 @@
     <t>AAS90021.1 (0.0)</t>
   </si>
   <si>
-    <t>oxidoreductase AflY (1.2563695321631984E-281)</t>
-  </si>
-  <si>
-    <t>oxidoreductase AflX (4.40471016040246E-159)</t>
-  </si>
-  <si>
-    <t>hydroxyversicolorone monooxygenase [EC:1.14.13.-] (2.94665797521859E-299)</t>
-  </si>
-  <si>
-    <t>averufin monooxygenase [EC:1.14.-.-] (4.116009209315507E-284)</t>
+    <t>oxidoreductase AflY (7.166118566209732E-279)</t>
+  </si>
+  <si>
+    <t>oxidoreductase AflX (1.1043128448364658E-117)</t>
+  </si>
+  <si>
+    <t>hydroxyversicolorone monooxygenase [EC:1.14.13.-] (3.3946231721094326E-300)</t>
+  </si>
+  <si>
+    <t>averufin monooxygenase [EC:1.14.-.-] (2.01197601405905E-277)</t>
   </si>
   <si>
     <t>5'-oxoaverantin cyclase / versicolorin B synthase [EC:4.2.1.142 4.2.1.143] (0.0)</t>
@@ -296,40 +296,40 @@
     <t>aflatoxin B synthase [EC:1.14.14.117] (0.0)</t>
   </si>
   <si>
-    <t>sterigmatocystin 8-O-methyltransferase [EC:2.1.1.110] (2.1778167877694904E-224)</t>
-  </si>
-  <si>
-    <t>demethylsterigmatocystin 6-O-methyltransferase [EC:2.1.1.109] (1.2513260582334386E-180)</t>
-  </si>
-  <si>
-    <t>oxidoreductase AflX (1.4381256538903229E-39)</t>
-  </si>
-  <si>
-    <t>noranthrone monooxygenase [EC:1.13.12.20] (1.5336150899952146E-47)</t>
-  </si>
-  <si>
-    <t>versicolorin B desaturase [EC:1.14.-.-] (1.7683268341563795E-286)</t>
-  </si>
-  <si>
-    <t>averantin hydroxylase [EC:1.14.14.116] (5.97332933782403E-303)</t>
-  </si>
-  <si>
-    <t>sterigmatocystin biosynthesis cytochrome P450 monooxygenase (2.4173668442045427E-284)</t>
-  </si>
-  <si>
-    <t>NADPH-dependent reductase (1.0539066011133975E-156)</t>
-  </si>
-  <si>
-    <t>1-deoxyxylulose-5-phosphate synthase [EC:1.1.-.-] (6.291050628132009E-82)</t>
-  </si>
-  <si>
-    <t>versiconal hemiacetal acetate esterase [EC:3.1.1.94] (2.6949659307667918E-126)</t>
-  </si>
-  <si>
-    <t>5'-hydroxyaverantin dehydrogenase [EC:1.1.1.352] (9.452111556343372E-168)</t>
-  </si>
-  <si>
-    <t>C6 transcription factor GliZ (6.622497571545114E-22)</t>
+    <t>sterigmatocystin 8-O-methyltransferase [EC:2.1.1.110] (2.190858608072448E-224)</t>
+  </si>
+  <si>
+    <t>demethylsterigmatocystin 6-O-methyltransferase [EC:2.1.1.109] (1.5507880480698545E-183)</t>
+  </si>
+  <si>
+    <t>oxidoreductase AflX (6.409364611182948E-41)</t>
+  </si>
+  <si>
+    <t>noranthrone monooxygenase [EC:1.13.12.20] (8.854556571746708E-48)</t>
+  </si>
+  <si>
+    <t>versicolorin B desaturase [EC:1.14.-.-] (3.102772686478476E-283)</t>
+  </si>
+  <si>
+    <t>averantin hydroxylase [EC:1.14.14.116] (6.694631299264637E-294)</t>
+  </si>
+  <si>
+    <t>sterigmatocystin biosynthesis cytochrome P450 monooxygenase (3.858531896224382E-276)</t>
+  </si>
+  <si>
+    <t>NADPH-dependent reductase (7.421789017761743E-155)</t>
+  </si>
+  <si>
+    <t>1-deoxyxylulose-5-phosphate synthase [EC:1.1.-.-] (1.9430995586336887E-82)</t>
+  </si>
+  <si>
+    <t>versiconal hemiacetal acetate esterase [EC:3.1.1.94] (1.0754281079871653E-126)</t>
+  </si>
+  <si>
+    <t>5'-hydroxyaverantin dehydrogenase [EC:1.1.1.352] (5.8934899442965265E-167)</t>
+  </si>
+  <si>
+    <t>C6 transcription factor GliZ (6.662156290207726E-22)</t>
   </si>
   <si>
     <t>fatty acid synthase subunit beta, fungi type [EC:2.3.1.86] (0.0)</t>
@@ -338,76 +338,85 @@
     <t>fatty acid synthase subunit alpha, fungi type [EC:2.3.1.86] (0.0)</t>
   </si>
   <si>
-    <t>norsolorinic acid ketoreductase [EC:1.1.1.349] (2.1003650551057863E-103)</t>
-  </si>
-  <si>
-    <t>noranthrone monooxygenase [EC:1.13.12.20] (1.695223790628791E-89)</t>
+    <t>norsolorinic acid ketoreductase [EC:1.1.1.349] (4.288328352449517E-102)</t>
+  </si>
+  <si>
+    <t>noranthrone monooxygenase [EC:1.13.12.20] (1.069426962885018E-86)</t>
   </si>
   <si>
     <t>noranthrone synthase [EC:2.3.1.221] (0.0)</t>
   </si>
   <si>
-    <t>MFS transporter, DHA2 family, glioxin efflux transporter (1.1637021821531554E-172)</t>
-  </si>
-  <si>
-    <t>thromboxane-A synthase [EC:5.3.99.5] (1.5441155608340824E-23)</t>
-  </si>
-  <si>
-    <t>ArsO family NAD(P)H-dependent flavin-containing monooxygenase (1.1830462757691442E-13)</t>
-  </si>
-  <si>
-    <t>cytochrome P450, cyclodipeptide synthase-associated (5.537401396682527E-7)</t>
-  </si>
-  <si>
-    <t>choline dehydrogenase (5.45468157597664E-96)</t>
-  </si>
-  <si>
-    <t>C-20 methyltransferase BchU (0.0000035326496620582435)</t>
-  </si>
-  <si>
-    <t>C-20 methyltransferase BchU (0.0000024596586014855904)</t>
-  </si>
-  <si>
-    <t>cytochrome P450, cyclodipeptide synthase-associated (4.166206739132496E-8)</t>
-  </si>
-  <si>
-    <t>EthD family reductase (1.8679676103337763E-8)</t>
-  </si>
-  <si>
-    <t>glucose 1-dehydrogenase (1.3216862422114519E-65)</t>
-  </si>
-  <si>
-    <t>NADP(H)-dependent aldo-keto reductase (4.269325938492079E-27)</t>
-  </si>
-  <si>
-    <t>chloramphenicol hydrolase (4.431944800119048E-30)</t>
-  </si>
-  <si>
-    <t>SDR family oxidoreductase (2.2290243961872364E-24)</t>
-  </si>
-  <si>
-    <t>ACP S-malonyltransferase (2.650092382995178E-26)</t>
-  </si>
-  <si>
-    <t>beta-ketoacyl-ACP synthase II (3.225879651928942E-29)</t>
-  </si>
-  <si>
-    <t>SDR family oxidoreductase (2.176311398196359E-19)</t>
-  </si>
-  <si>
-    <t>polyketide synthase Pks13 (4.854412606563152E-162)</t>
-  </si>
-  <si>
-    <t>DHA2 family efflux MFS transporter permease subunit (4.740953083637269E-52)</t>
-  </si>
-  <si>
-    <t>cytochrome P450, cyclodipeptide synthase-associated (0.0000023506716319589886)</t>
+    <t>MFS transporter, DHA2 family, glioxin efflux transporter (3.0143414956217645E-173)</t>
+  </si>
+  <si>
+    <t>cytochrome P450 family 3 subfamily A [EC:1.14.14.1] (9.239801302352214E-24)</t>
+  </si>
+  <si>
+    <t>neopentalenolactone/pentalenolactone D synthase (6.317096337029139E-45)</t>
+  </si>
+  <si>
+    <t>pentalenene oxygenase (1.201132374574542E-15)</t>
+  </si>
+  <si>
+    <t>choline dehydrogenase (5.549238712494822E-96)</t>
+  </si>
+  <si>
+    <t>pentalenene oxygenase (1.031009914121179E-10)</t>
+  </si>
+  <si>
+    <t>bacteriochlorophyllide d C-20 methyltransferase BchU (0.0000035938882938121676)</t>
+  </si>
+  <si>
+    <t>bacteriochlorophyllide d C-20 methyltransferase BchU (0.0000025022968876860365)</t>
+  </si>
+  <si>
+    <t>pentalenene oxygenase (5.619143134625434E-14)</t>
+  </si>
+  <si>
+    <t>pentalenene oxygenase (7.937639638561679E-17)</t>
+  </si>
+  <si>
+    <t>pentalenene oxygenase (2.2210214218559466E-19)</t>
+  </si>
+  <si>
+    <t>EthD family reductase (1.900348908101877E-8)</t>
+  </si>
+  <si>
+    <t>glucose 1-dehydrogenase (1.3445977292887915E-65)</t>
+  </si>
+  <si>
+    <t>NADP(H)-dependent aldo-keto reductase (4.343334884749282E-27)</t>
+  </si>
+  <si>
+    <t>chloramphenicol hydrolase (4.508772751241176E-30)</t>
+  </si>
+  <si>
+    <t>SDR family oxidoreductase (2.267664628654866E-24)</t>
+  </si>
+  <si>
+    <t>ACP S-malonyltransferase (2.696031846876679E-26)</t>
+  </si>
+  <si>
+    <t>beta-ketoacyl-ACP synthase II (3.28180041254347E-29)</t>
+  </si>
+  <si>
+    <t>SDR family oxidoreductase (2.2140378486076246E-19)</t>
+  </si>
+  <si>
+    <t>polyketide synthase Pks13 (4.938564055031926E-162)</t>
+  </si>
+  <si>
+    <t>DHA2 family efflux MFS transporter permease subunit (4.8231377064629415E-52)</t>
+  </si>
+  <si>
+    <t>pentalenene oxygenase (1.170148979535974E-10)</t>
   </si>
   <si>
     <t>Q6UEF1 (0.0)</t>
   </si>
   <si>
-    <t>metacyc::MONOMER-21284 (5.07E-209)</t>
+    <t>metacyc::MONOMER-21284 (5.14E-209)</t>
   </si>
   <si>
     <t>Q6UEF3 (0.0)</t>
@@ -422,16 +431,16 @@
     <t>SwissProt::B8NHY4 (0.0)</t>
   </si>
   <si>
-    <t>Q5VDD7 (1.28E-300)</t>
-  </si>
-  <si>
-    <t>Q9P900 (1.58E-269)</t>
-  </si>
-  <si>
-    <t>SwissProt::Q9P8Z9 (3.70E-182)</t>
-  </si>
-  <si>
-    <t>SwissProt::B8NI03 (1.13E-28)</t>
+    <t>Q5VDD7 (1.30E-300)</t>
+  </si>
+  <si>
+    <t>Q9P900 (1.60E-269)</t>
+  </si>
+  <si>
+    <t>SwissProt::Q9P8Z9 (3.75E-182)</t>
+  </si>
+  <si>
+    <t>SwissProt::B8NI03 (1.15E-28)</t>
   </si>
   <si>
     <t>B8NHY9 (0.0)</t>
@@ -440,28 +449,28 @@
     <t>ENA::AAS90101.1 (0.0)</t>
   </si>
   <si>
-    <t>XP_001219467.1 (1.68E-48)</t>
+    <t>XP_001219467.1 (1.71E-48)</t>
   </si>
   <si>
     <t>B8NHZ2 (0.0)</t>
   </si>
   <si>
-    <t>B8NHZ4 (4.10E-185)</t>
-  </si>
-  <si>
-    <t>Q00258 (1.28E-283)</t>
-  </si>
-  <si>
-    <t>B8NHZ6 (6.64E-242)</t>
-  </si>
-  <si>
-    <t>B8NHZ7 (5.78E-223)</t>
-  </si>
-  <si>
-    <t>ENA::AAS90096.1 (2.34E-307)</t>
-  </si>
-  <si>
-    <t>SwissProt::P41765 (4.67E-301)</t>
+    <t>B8NHZ4 (4.15E-185)</t>
+  </si>
+  <si>
+    <t>Q00258 (1.30E-283)</t>
+  </si>
+  <si>
+    <t>B8NHZ6 (6.73E-242)</t>
+  </si>
+  <si>
+    <t>B8NHZ7 (5.86E-223)</t>
+  </si>
+  <si>
+    <t>ENA::AAS90096.1 (2.38E-307)</t>
+  </si>
+  <si>
+    <t>SwissProt::P41765 (4.73E-301)</t>
   </si>
   <si>
     <t>Q5VDA1 (0.0)</t>
@@ -470,10 +479,10 @@
     <t>Q5VDA2 (0.0)</t>
   </si>
   <si>
-    <t>B8NI02 (1.55E-202)</t>
-  </si>
-  <si>
-    <t>SwissProt::B8NI03 (1.23E-146)</t>
+    <t>B8NI02 (1.57E-202)</t>
+  </si>
+  <si>
+    <t>SwissProt::B8NI03 (1.25E-146)</t>
   </si>
   <si>
     <t>Q5VDF2 (0.0)</t>
@@ -482,13 +491,13 @@
     <t>Q6UEH3 (0.0)</t>
   </si>
   <si>
-    <t>Q6UEH4 (6.74E-145)</t>
+    <t>Q6UEH4 (6.83E-145)</t>
   </si>
   <si>
     <t>gb|BAB43261.1|ARO:3007013|sdrM [Staphylococcus aureus subsp. aureus N315] (3.67E-27)</t>
   </si>
   <si>
-    <t>BGC0000010|c1|67004-68604|-|AAS90089.1|HypA|AAS90089.1; BGC0000006|c1|75783-77383|-|AAS90113.1|hypothetical_protein|AAS90113.1 (0.0)</t>
+    <t>BGC0000006|c1|75783-77383|-|AAS90113.1|hypothetical_protein|AAS90113.1; BGC0000010|c1|67004-68604|-|AAS90089.1|HypA|AAS90089.1 (0.0)</t>
   </si>
   <si>
     <t>BGC0000010|c1|65849-66649|-|AAS90084.1|OrdB|AAS90084.1 (3.74E-193)</t>
@@ -533,13 +542,13 @@
     <t>BGC0000011|c1|8002-8397|-|ACH72914.1|HypE|ACH72914.1 (4.84E-61)</t>
   </si>
   <si>
-    <t>BGC0000007|c1|52798-53697|+|AAS90008.1|Ver-1|AAS90008.1; BGC0000008|c1|41518-42418|+|AAS90030.1|Ver-1|AAS90030.1 (3.07E-186)</t>
+    <t>BGC0000008|c1|41518-42418|+|AAS90030.1|Ver-1|AAS90030.1; BGC0000007|c1|52798-53697|+|AAS90008.1|Ver-1|AAS90008.1 (3.07E-186)</t>
   </si>
   <si>
     <t>BGC0000006|c1|47807-49091|+|AAS90094.1|NorA|AAS90094.1; BGC0000010|c1|39072-40356|+|AAS90074.1|NorA|AAS90074.1 (2.20E-290)</t>
   </si>
   <si>
-    <t>BGC0000006|c1|46515-47516|+|AAS90098.1|EstA|AAS90098.1; BGC0000008|c1|38128-39129|+|AAS90029.1|EstA|AAS90029.1 (4.98E-243)</t>
+    <t>BGC0000008|c1|38128-39129|+|AAS90029.1|EstA|AAS90029.1; BGC0000006|c1|46515-47516|+|AAS90098.1|EstA|AAS90098.1 (4.98E-243)</t>
   </si>
   <si>
     <t>BGC0000011|c1|32719-32997|-|ACH72903.1|StcH|ACH72903.1 (4.01E-30)</t>
@@ -551,13 +560,13 @@
     <t>BGC0000008|c1|34339-35800|+|AAS90027.1|AflJ|AAS90027.1 (1.51E-309)</t>
   </si>
   <si>
-    <t>BGC0000008|c1|32264-33598|-|AAS90026.1|AflR|AAS90026.1; BGC0000010|c1|31932-33266|-|AAS90086.1|AflR|AAS90086.1; BGC0000006|c1|40669-42003|-|AAS90091.1|AflR|AAS90091.1 (8.59E-303)</t>
+    <t>BGC0000010|c1|31932-33266|-|AAS90086.1|AflR|AAS90086.1; BGC0000008|c1|32264-33598|-|AAS90026.1|AflR|AAS90026.1; BGC0000006|c1|40669-42003|-|AAS90091.1|AflR|AAS90091.1 (8.59E-303)</t>
   </si>
   <si>
     <t>BGC0000006|c1|33553-39399|+|AAS90095.1|Fas-1/HexB|AAS90095.1 (0.0)</t>
   </si>
   <si>
-    <t>BGC0000008|c1|19319-24439|-|AAS90024.1|HexA|AAS90024.1; BGC0000006|c1|27719-32839|-|AAS90111.1|Fas-2/HexA|AAS90111.1 (0.0)</t>
+    <t>BGC0000006|c1|27719-32839|-|AAS90111.1|Fas-2/HexA|AAS90111.1; BGC0000008|c1|19319-24439|-|AAS90024.1|HexA|AAS90024.1 (0.0)</t>
   </si>
   <si>
     <t>BGC0000010|c1|16690-17679|+|AAS90070.1|Nor-1|AAS90070.1 (2.58E-189)</t>
@@ -575,43 +584,40 @@
     <t>BGC0000007|c1|13721-15482|+|AAS89997.1|CypA|AAS89997.1 (1.23E-118)</t>
   </si>
   <si>
-    <t>sp|Q5URB2|YR188_MIMIV Uncharacterized protein R188[Xs] (1.2949111647966325E-7)</t>
-  </si>
-  <si>
-    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (1.9195016967058424E-23)</t>
-  </si>
-  <si>
-    <t>sp|Q5UPL2|YR135_MIMIV Putative GMC-type oxidoreductase R135[XhXs] (8.165434609163075E-89)</t>
-  </si>
-  <si>
-    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (9.163547384092897E-28)</t>
-  </si>
-  <si>
-    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (1.1970462578275103E-27)</t>
-  </si>
-  <si>
-    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (2.1919143449083863E-33)</t>
-  </si>
-  <si>
-    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (1.3592831436655338E-31)</t>
-  </si>
-  <si>
-    <t>sp|P37079|SORD_KLEPN Sorbitol-6-phosphate 2-dehydrogenase[Xh] (1.808313592449771E-36)</t>
-  </si>
-  <si>
-    <t>sp|O64252|PRXH_BPMD2 Putative non-heme haloperoxidase[Xh] (1.22891785331551E-9)</t>
-  </si>
-  <si>
-    <t>sp|P37079|SORD_KLEPN Sorbitol-6-phosphate 2-dehydrogenase[Xh] (1.9449278910062017E-16)</t>
-  </si>
-  <si>
-    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (1.572399079898436E-17)</t>
+    <t>sp|O48786|C734A_ARATH Cytochrome P450 734A1[Xh] (5.314492165360873E-13)</t>
+  </si>
+  <si>
+    <t>sp|Q9WWW2|ALKJ_PSEPU Alcohol dehydrogenase [acceptor][Xh] (1.6754300581320288E-66)</t>
+  </si>
+  <si>
+    <t>sp|P98187|CP4F8_HUMAN Cytochrome P450 4F8[Xh] (1.224118370913633E-14)</t>
+  </si>
+  <si>
+    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (2.3485373520488118E-18)</t>
+  </si>
+  <si>
+    <t>sp|Q5UQ90|YL532_MIMIV Cytochrome P450-like protein L532[XhXs] (5.333347591333469E-24)</t>
+  </si>
+  <si>
+    <t>sp|P98187|CP4F8_HUMAN Cytochrome P450 4F8[Xh] (7.794127130526876E-28)</t>
+  </si>
+  <si>
+    <t>sp|P37079|SORD_KLEPN Sorbitol-6-phosphate 2-dehydrogenase[Xh] (1.284129490128239E-38)</t>
+  </si>
+  <si>
+    <t>sp|Q5UQ83|YR526_MIMIV Putative alpha/beta hydrolase R526[Xs] (4.7425570647592076E-23)</t>
+  </si>
+  <si>
+    <t>sp|P37079|SORD_KLEPN Sorbitol-6-phosphate 2-dehydrogenase[Xh] (2.2345903911841373E-16)</t>
+  </si>
+  <si>
+    <t>sp|P98187|CP4F8_HUMAN Cytochrome P450 4F8[Xh] (1.1943517745771795E-8)</t>
   </si>
   <si>
     <t>VFG005765(gb|WP_000861303) (cylG) 3-ketoacyl-ACP-reductase CylG [-haemolysin/cytolysin (VF0279) - Exotoxin (VFC0235)] [Streptococcus agalactiae A909]; VFG005766(gb|WP_000861302) (cylG) 3-ketoacyl-ACP-reductase CylG [Beta-haemolysin/cytolysin (VF0279) - Exotoxin (VFC0235)] [Streptococcus agalactiae NEM316] (7.95E-30)</t>
   </si>
   <si>
-    <t>VFG009414(gb|WP_173812288) (mlsB) SDR family NAD(P)-dependent oxidoreductase [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium ulcerans Agy99]; VFG009412(gb|WP_011178521) (mlsA1) SDR family NAD(P)-dependent oxidoreductase [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium ulcerans Agy99]; VFG026440(gb|ACA57625) (mlsA1) type I modular polyketide synthase, MlsA1 [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium liflandii 128FXT]; VFG026442(gb|ACA57618) (mlsB) type I modular polyketide synthase, MlsB [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium liflandii 128FXT] (0.00000221)</t>
+    <t>VFG009412(gb|WP_011178521) (mlsA1) SDR family NAD(P)-dependent oxidoreductase [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium ulcerans Agy99]; VFG009414(gb|WP_173812288) (mlsB) SDR family NAD(P)-dependent oxidoreductase [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium ulcerans Agy99]; VFG026442(gb|ACA57618) (mlsB) type I modular polyketide synthase, MlsB [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium liflandii 128FXT]; VFG026440(gb|ACA57625) (mlsA1) type I modular polyketide synthase, MlsA1 [Mycolactone (VF0817) - Exotoxin (VFC0235)] [Mycobacterium liflandii 128FXT] (0.00000221)</t>
   </si>
   <si>
     <t>VFG029825(gb|WP_041309443) (pks) type I polyketide synthase [GPL locus (VF0841) - Immune modulation (VFC0258)] [Mycobacterium sp. KMS] (8.26E-137)</t>
@@ -1449,7 +1455,7 @@
         <v>62</v>
       </c>
       <c r="T2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="U2" t="s">
         <v>62</v>
@@ -1458,7 +1464,7 @@
         <v>62</v>
       </c>
       <c r="W2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="X2" t="s">
         <v>62</v>
@@ -1467,13 +1473,13 @@
         <v>62</v>
       </c>
       <c r="Z2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AA2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AB2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -1535,7 +1541,7 @@
         <v>62</v>
       </c>
       <c r="T3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="U3" t="s">
         <v>62</v>
@@ -1544,7 +1550,7 @@
         <v>62</v>
       </c>
       <c r="W3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="X3" t="s">
         <v>62</v>
@@ -1553,13 +1559,13 @@
         <v>62</v>
       </c>
       <c r="Z3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AA3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AB3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -1621,7 +1627,7 @@
         <v>111</v>
       </c>
       <c r="T4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="U4" t="s">
         <v>62</v>
@@ -1630,22 +1636,22 @@
         <v>62</v>
       </c>
       <c r="W4" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="X4" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
       <c r="Y4" t="s">
         <v>62</v>
       </c>
       <c r="Z4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AA4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AB4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -1707,7 +1713,7 @@
         <v>112</v>
       </c>
       <c r="T5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="U5" t="s">
         <v>62</v>
@@ -1716,22 +1722,22 @@
         <v>62</v>
       </c>
       <c r="W5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="X5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y5" t="s">
         <v>62</v>
       </c>
       <c r="Z5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AB5" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -1793,7 +1799,7 @@
         <v>113</v>
       </c>
       <c r="T6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="U6" t="s">
         <v>62</v>
@@ -1802,22 +1808,22 @@
         <v>62</v>
       </c>
       <c r="W6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="X6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y6" t="s">
         <v>62</v>
       </c>
       <c r="Z6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AA6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="AB6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -1876,10 +1882,10 @@
         <v>91</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="T7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="U7" t="s">
         <v>62</v>
@@ -1888,22 +1894,22 @@
         <v>62</v>
       </c>
       <c r="W7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="X7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="Y7" t="s">
         <v>62</v>
       </c>
       <c r="Z7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="AB7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -1962,10 +1968,10 @@
         <v>92</v>
       </c>
       <c r="S8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="T8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="U8" t="s">
         <v>62</v>
@@ -1974,7 +1980,7 @@
         <v>62</v>
       </c>
       <c r="W8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="X8" t="s">
         <v>62</v>
@@ -1983,13 +1989,13 @@
         <v>62</v>
       </c>
       <c r="Z8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AA8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AB8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -2048,10 +2054,10 @@
         <v>93</v>
       </c>
       <c r="S9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="U9" t="s">
         <v>62</v>
@@ -2060,7 +2066,7 @@
         <v>62</v>
       </c>
       <c r="W9" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="X9" t="s">
         <v>62</v>
@@ -2069,13 +2075,13 @@
         <v>62</v>
       </c>
       <c r="Z9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AA9" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AB9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:28">
@@ -2137,7 +2143,7 @@
         <v>62</v>
       </c>
       <c r="T10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="U10" t="s">
         <v>62</v>
@@ -2146,7 +2152,7 @@
         <v>62</v>
       </c>
       <c r="W10" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="X10" t="s">
         <v>62</v>
@@ -2155,13 +2161,13 @@
         <v>62</v>
       </c>
       <c r="Z10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AA10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AB10" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -2223,7 +2229,7 @@
         <v>62</v>
       </c>
       <c r="T11" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U11" t="s">
         <v>62</v>
@@ -2232,7 +2238,7 @@
         <v>62</v>
       </c>
       <c r="W11" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="X11" t="s">
         <v>62</v>
@@ -2241,13 +2247,13 @@
         <v>62</v>
       </c>
       <c r="Z11" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AA11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AB11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:28">
@@ -2306,10 +2312,10 @@
         <v>96</v>
       </c>
       <c r="S12" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="T12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="U12" t="s">
         <v>62</v>
@@ -2318,22 +2324,22 @@
         <v>62</v>
       </c>
       <c r="W12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="X12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="Y12" t="s">
         <v>62</v>
       </c>
       <c r="Z12" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA12" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AB12" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -2392,10 +2398,10 @@
         <v>97</v>
       </c>
       <c r="S13" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="T13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="U13" t="s">
         <v>62</v>
@@ -2404,22 +2410,22 @@
         <v>62</v>
       </c>
       <c r="W13" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="X13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="Y13" t="s">
         <v>62</v>
       </c>
       <c r="Z13" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA13" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AB13" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:28">
@@ -2481,7 +2487,7 @@
         <v>62</v>
       </c>
       <c r="T14" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U14" t="s">
         <v>62</v>
@@ -2490,7 +2496,7 @@
         <v>62</v>
       </c>
       <c r="W14" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="X14" t="s">
         <v>62</v>
@@ -2499,13 +2505,13 @@
         <v>62</v>
       </c>
       <c r="Z14" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AA14" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AB14" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:28">
@@ -2564,10 +2570,10 @@
         <v>98</v>
       </c>
       <c r="S15" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="T15" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="U15" t="s">
         <v>62</v>
@@ -2576,22 +2582,22 @@
         <v>62</v>
       </c>
       <c r="W15" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="X15" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Y15" t="s">
         <v>62</v>
       </c>
       <c r="Z15" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA15" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AB15" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -2650,7 +2656,7 @@
         <v>62</v>
       </c>
       <c r="S16" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="T16" t="s">
         <v>62</v>
@@ -2662,7 +2668,7 @@
         <v>62</v>
       </c>
       <c r="W16" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="X16" t="s">
         <v>62</v>
@@ -2671,13 +2677,13 @@
         <v>62</v>
       </c>
       <c r="Z16" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AA16" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AB16" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -2736,10 +2742,10 @@
         <v>99</v>
       </c>
       <c r="S17" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="T17" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="U17" t="s">
         <v>62</v>
@@ -2748,22 +2754,22 @@
         <v>62</v>
       </c>
       <c r="W17" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="X17" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Y17" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="Z17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AA17" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AB17" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:28">
@@ -2822,10 +2828,10 @@
         <v>100</v>
       </c>
       <c r="S18" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="T18" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="U18" t="s">
         <v>62</v>
@@ -2834,7 +2840,7 @@
         <v>62</v>
       </c>
       <c r="W18" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="X18" t="s">
         <v>62</v>
@@ -2843,13 +2849,13 @@
         <v>62</v>
       </c>
       <c r="Z18" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AA18" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AB18" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:28">
@@ -2908,10 +2914,10 @@
         <v>101</v>
       </c>
       <c r="S19" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="T19" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="U19" t="s">
         <v>62</v>
@@ -2920,22 +2926,22 @@
         <v>62</v>
       </c>
       <c r="W19" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="X19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="Y19" t="s">
         <v>62</v>
       </c>
       <c r="Z19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AA19" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AB19" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:28">
@@ -3006,7 +3012,7 @@
         <v>62</v>
       </c>
       <c r="W20" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="X20" t="s">
         <v>62</v>
@@ -3015,13 +3021,13 @@
         <v>62</v>
       </c>
       <c r="Z20" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="AA20" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AB20" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:28">
@@ -3080,10 +3086,10 @@
         <v>102</v>
       </c>
       <c r="S21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="T21" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="U21" t="s">
         <v>62</v>
@@ -3092,22 +3098,22 @@
         <v>62</v>
       </c>
       <c r="W21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="X21" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="Y21" t="s">
         <v>62</v>
       </c>
       <c r="Z21" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="AA21" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AB21" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:28">
@@ -3169,7 +3175,7 @@
         <v>62</v>
       </c>
       <c r="T22" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="U22" t="s">
         <v>62</v>
@@ -3178,7 +3184,7 @@
         <v>62</v>
       </c>
       <c r="W22" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="X22" t="s">
         <v>62</v>
@@ -3190,10 +3196,10 @@
         <v>62</v>
       </c>
       <c r="AA22" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AB22" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:28">
@@ -3255,7 +3261,7 @@
         <v>62</v>
       </c>
       <c r="T23" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="U23" t="s">
         <v>62</v>
@@ -3264,7 +3270,7 @@
         <v>62</v>
       </c>
       <c r="W23" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="X23" t="s">
         <v>62</v>
@@ -3273,13 +3279,13 @@
         <v>62</v>
       </c>
       <c r="Z23" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AA23" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AB23" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:28">
@@ -3338,10 +3344,10 @@
         <v>104</v>
       </c>
       <c r="S24" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="T24" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="U24" t="s">
         <v>62</v>
@@ -3350,22 +3356,22 @@
         <v>62</v>
       </c>
       <c r="W24" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="X24" t="s">
         <v>62</v>
       </c>
       <c r="Y24" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="Z24" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AA24" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="AB24" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:28">
@@ -3424,10 +3430,10 @@
         <v>105</v>
       </c>
       <c r="S25" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="T25" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="U25" t="s">
         <v>62</v>
@@ -3436,7 +3442,7 @@
         <v>62</v>
       </c>
       <c r="W25" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="X25" t="s">
         <v>62</v>
@@ -3445,13 +3451,13 @@
         <v>62</v>
       </c>
       <c r="Z25" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AA25" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AB25" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:28">
@@ -3510,10 +3516,10 @@
         <v>106</v>
       </c>
       <c r="S26" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T26" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="U26" t="s">
         <v>62</v>
@@ -3522,7 +3528,7 @@
         <v>62</v>
       </c>
       <c r="W26" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="X26" t="s">
         <v>62</v>
@@ -3531,13 +3537,13 @@
         <v>62</v>
       </c>
       <c r="Z26" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="AA26" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AB26" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:28">
@@ -3599,7 +3605,7 @@
         <v>62</v>
       </c>
       <c r="T27" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="U27" t="s">
         <v>62</v>
@@ -3608,7 +3614,7 @@
         <v>62</v>
       </c>
       <c r="W27" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="X27" t="s">
         <v>62</v>
@@ -3617,13 +3623,13 @@
         <v>62</v>
       </c>
       <c r="Z27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AA27" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AB27" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -3682,10 +3688,10 @@
         <v>108</v>
       </c>
       <c r="S28" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="T28" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="U28" t="s">
         <v>62</v>
@@ -3694,22 +3700,22 @@
         <v>62</v>
       </c>
       <c r="W28" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="X28" t="s">
         <v>62</v>
       </c>
       <c r="Y28" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z28" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AA28" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB28" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:28">
@@ -3768,34 +3774,34 @@
         <v>109</v>
       </c>
       <c r="S29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="T29" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="U29" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="V29" t="s">
         <v>62</v>
       </c>
       <c r="W29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="X29" t="s">
         <v>62</v>
       </c>
       <c r="Y29" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Z29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="AA29" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AB29" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:28">
@@ -3854,10 +3860,10 @@
         <v>110</v>
       </c>
       <c r="S30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="T30" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="U30" t="s">
         <v>62</v>
@@ -3866,22 +3872,22 @@
         <v>62</v>
       </c>
       <c r="W30" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="X30" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="Y30" t="s">
         <v>62</v>
       </c>
       <c r="Z30" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AA30" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AB30" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>